<commit_message>
feat(config): add Pembro status clinical variable
Add Pembro_status to clinical variables with three treatment
line categories (Front-line, Second-line, Third-line) and
corresponding color scheme. Update clinical variables list
and UMAP marker plotting configuration.

Changes:
- Add Pembro_status to `clinVars_Lung.txt`
- Define color palette for Pembro_status treatment lines in
  `global_plot_colors.yaml`
- Update `umap_marker_plotting_Lung.xlsx` configuration

Co-Authored-By: Claude
</commit_message>
<xml_diff>
--- a/assets/graphics/umap_marker_plotting_Lung.xlsx
+++ b/assets/graphics/umap_marker_plotting_Lung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pourmalm/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pourmalm/Documents/Work/Mellinghoff_lab/Data/nsclc/NSCLC_MetaData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91043FCB-509B-4A46-8D8E-C1923DAE5594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42892E9-6B77-8647-9ABC-D49189BD8C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33560" yWindow="1880" windowWidth="14400" windowHeight="17120" xr2:uid="{C98B34FD-B8C4-8D46-9A0E-B0A523AB0124}"/>
+    <workbookView xWindow="12920" yWindow="500" windowWidth="15880" windowHeight="16660" xr2:uid="{C98B34FD-B8C4-8D46-9A0E-B0A523AB0124}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>CD45</t>
   </si>
@@ -213,13 +213,52 @@
     <t>Metastasis_brain</t>
   </si>
   <si>
-    <t>Metastasis_multiple</t>
-  </si>
-  <si>
-    <t>Best_overall_response_abbrev</t>
-  </si>
-  <si>
     <t>PDL1_percent_score_group</t>
+  </si>
+  <si>
+    <t>Pembro_status</t>
+  </si>
+  <si>
+    <t>Sample_type</t>
+  </si>
+  <si>
+    <t>Body_part</t>
+  </si>
+  <si>
+    <t>Body_part_abbrev</t>
+  </si>
+  <si>
+    <t>Metastasis_brain_status</t>
+  </si>
+  <si>
+    <t>predictive_biomarker</t>
+  </si>
+  <si>
+    <t>Best_overall_response_group</t>
+  </si>
+  <si>
+    <t>Best_overall_response_detailed</t>
+  </si>
+  <si>
+    <t>PFS_months_group_median</t>
+  </si>
+  <si>
+    <t>PFS_months_group_quartile</t>
+  </si>
+  <si>
+    <t>OS_months_group_median</t>
+  </si>
+  <si>
+    <t>OS_months_group_quartile</t>
+  </si>
+  <si>
+    <t>Impact_TMB_score_group10</t>
+  </si>
+  <si>
+    <t>STK11</t>
+  </si>
+  <si>
+    <t>KEAP1</t>
   </si>
 </sst>
 </file>
@@ -255,9 +294,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +617,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
@@ -593,7 +631,7 @@
       <c r="A1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>31</v>
       </c>
       <c r="C1" t="s">
@@ -607,229 +645,268 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(config): update clinical variables and colors
Add Sample_pretreated clinical variable with three treatment
categories (Systemic, Radiation, N) and corresponding color
scheme. Update PDL1 variable name from PDL1_percent_score_group
to PDL1_IHC_percent_DrYang_group with revised color palette
(orange tones) and add NA category. Change Lung body part
color from blue to magenta for better visual distinction.

Changes:
- Add Sample_pretreated to clinical variables list
- Add Sample_pretreated color mappings (brown/orange/light blue)
- Rename PDL1_percent_score_group to PDL1_IHC_percent_DrYang_group
- Update PDL1 colors (high: orange, low: peach, NA: gray)
- Update Lung/Body_part_abbrev colors from blue to magenta
- Update UMAP marker plotting configuration file

Co-Authored-By: Claude
</commit_message>
<xml_diff>
--- a/assets/graphics/umap_marker_plotting_Lung.xlsx
+++ b/assets/graphics/umap_marker_plotting_Lung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pourmalm/Documents/Work/Mellinghoff_lab/Data/nsclc/NSCLC_MetaData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42892E9-6B77-8647-9ABC-D49189BD8C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791A41DD-5B43-8444-AEA2-984326E63F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12920" yWindow="500" windowWidth="15880" windowHeight="16660" xr2:uid="{C98B34FD-B8C4-8D46-9A0E-B0A523AB0124}"/>
+    <workbookView xWindow="12920" yWindow="500" windowWidth="15880" windowHeight="16620" xr2:uid="{C98B34FD-B8C4-8D46-9A0E-B0A523AB0124}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>CD45</t>
   </si>
@@ -213,9 +213,6 @@
     <t>Metastasis_brain</t>
   </si>
   <si>
-    <t>PDL1_percent_score_group</t>
-  </si>
-  <si>
     <t>Pembro_status</t>
   </si>
   <si>
@@ -259,6 +256,12 @@
   </si>
   <si>
     <t>KEAP1</t>
+  </si>
+  <si>
+    <t>PDL1_IHC_percent_DrYang_group</t>
+  </si>
+  <si>
+    <t>Sample_pretreated</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
@@ -652,7 +655,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -666,7 +669,7 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -680,7 +683,7 @@
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -691,7 +694,7 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -702,7 +705,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -713,7 +716,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -724,7 +727,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -735,7 +738,7 @@
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -746,7 +749,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -757,7 +760,7 @@
         <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,7 +771,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -779,7 +782,7 @@
         <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -790,7 +793,7 @@
         <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -801,7 +804,7 @@
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -812,7 +815,7 @@
         <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -823,7 +826,7 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -834,7 +837,7 @@
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -842,7 +845,7 @@
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -850,7 +853,7 @@
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -858,7 +861,7 @@
         <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -866,7 +869,7 @@
         <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -874,7 +877,7 @@
         <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -882,12 +885,15 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>